<commit_message>
- add titles to all figures - check move speed and tiers correlation - add custom color map for p-value
</commit_message>
<xml_diff>
--- a/sc2 unit stats.xlsx
+++ b/sc2 unit stats.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="308">
   <si>
     <t>Probe</t>
   </si>
@@ -62,9 +63,6 @@
     <t>18.6 (+2.33)</t>
   </si>
   <si>
-    <t>3.15 (4.725 +5.67 C)</t>
-  </si>
-  <si>
     <t>Sentry</t>
   </si>
   <si>
@@ -125,9 +123,6 @@
     <t>1.61 (1.11)</t>
   </si>
   <si>
-    <t>3.5 (4.78)</t>
-  </si>
-  <si>
     <t>High Templar</t>
   </si>
   <si>
@@ -176,18 +171,12 @@
     <t>Observer</t>
   </si>
   <si>
-    <t>2.63 (+1.31)</t>
-  </si>
-  <si>
     <t>Warp Prism</t>
   </si>
   <si>
     <t>A, M, P</t>
   </si>
   <si>
-    <t>4.13 (5.36)</t>
-  </si>
-  <si>
     <t>Immortal</t>
   </si>
   <si>
@@ -260,9 +249,6 @@
     <t>+11.2, +28 A</t>
   </si>
   <si>
-    <t>3.85 (+0.798), (2.888 (-0.264)) [p 1]</t>
-  </si>
-  <si>
     <t>Oracle</t>
   </si>
   <si>
@@ -812,9 +798,6 @@
     <t>+3.8 A</t>
   </si>
   <si>
-    <t>0, 1.4</t>
-  </si>
-  <si>
     <t>x2.5</t>
   </si>
   <si>
@@ -963,6 +946,9 @@
   </si>
   <si>
     <t xml:space="preserve"> +0 (+0.7) L</t>
+  </si>
+  <si>
+    <t>Speed bonus</t>
   </si>
 </sst>
 </file>
@@ -1332,120 +1318,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y74"/>
+  <dimension ref="A1:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W67" sqref="W67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="2" customWidth="1"/>
     <col min="2" max="2" width="7" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.140625" style="2"/>
-    <col min="14" max="14" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" customWidth="1"/>
+    <col min="8" max="13" width="9.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="31.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11" style="2" customWidth="1"/>
+    <col min="21" max="21" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="2"/>
+    <col min="23" max="23" width="31.28515625" style="2" customWidth="1"/>
+    <col min="24" max="25" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="W1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="U1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>289</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
@@ -1504,22 +1494,23 @@
       <c r="V2" s="6">
         <v>3.94</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="W2" s="6"/>
+      <c r="Y2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Z2" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D3" s="6">
         <v>2</v>
@@ -1575,25 +1566,29 @@
       <c r="U3" s="6">
         <v>0.86</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="6">
+        <v>3.15</v>
+      </c>
+      <c r="W3" s="6">
+        <f>4.725-3.15</f>
+        <v>1.5749999999999997</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="B4" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D4" s="6">
         <v>2</v>
@@ -1605,7 +1600,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="6">
         <v>1</v>
@@ -1623,22 +1618,22 @@
         <v>40</v>
       </c>
       <c r="M4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>4</v>
@@ -1652,22 +1647,23 @@
       <c r="V4" s="6">
         <v>3.15</v>
       </c>
-      <c r="X4" s="6">
+      <c r="W4" s="6"/>
+      <c r="Y4" s="6">
         <v>5</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Z4" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D5" s="6">
         <v>2</v>
@@ -1679,7 +1675,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="6">
         <v>1.25</v>
@@ -1697,28 +1693,28 @@
         <v>80</v>
       </c>
       <c r="M5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="U5" s="6">
         <v>1.34</v>
@@ -1726,22 +1722,23 @@
       <c r="V5" s="6">
         <v>4.13</v>
       </c>
-      <c r="X5" s="6">
+      <c r="W5" s="6"/>
+      <c r="Y5" s="6">
         <v>6</v>
       </c>
-      <c r="Y5" s="6">
+      <c r="Z5" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D6" s="6">
         <v>2</v>
@@ -1753,7 +1750,7 @@
         <v>25</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -1774,48 +1771,52 @@
         <v>9</v>
       </c>
       <c r="N6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="R6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="S6" s="6" t="s">
+      <c r="T6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="T6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="U6" s="6" t="s">
+      <c r="V6" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="W6" s="6">
+        <f>4.78-3.5</f>
+        <v>1.2800000000000002</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="V6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X6" s="6">
-        <v>4</v>
-      </c>
-      <c r="Y6" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
@@ -1827,7 +1828,7 @@
         <v>150</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" s="6">
         <v>0.75</v>
@@ -1845,19 +1846,19 @@
         <v>40</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="R7" s="6" t="s">
         <v>4</v>
@@ -1874,22 +1875,23 @@
       <c r="V7" s="6">
         <v>2.62</v>
       </c>
-      <c r="X7" s="6">
+      <c r="W7" s="6"/>
+      <c r="Y7" s="6">
         <v>6</v>
       </c>
-      <c r="Y7" s="6">
+      <c r="Z7" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -1901,7 +1903,7 @@
         <v>125</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H8" s="6">
         <v>0.75</v>
@@ -1919,10 +1921,10 @@
         <v>80</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>4</v>
@@ -1931,7 +1933,7 @@
         <v>4</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R8" s="6" t="s">
         <v>4</v>
@@ -1948,22 +1950,23 @@
       <c r="V8" s="6">
         <v>3.94</v>
       </c>
-      <c r="X8" s="6" t="s">
+      <c r="W8" s="6"/>
+      <c r="Y8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Y8" s="6">
+      <c r="Z8" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D9" s="6">
         <v>4</v>
@@ -1993,28 +1996,28 @@
         <v>350</v>
       </c>
       <c r="M9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="Q9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="R9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="T9" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="U9" s="6">
         <v>1.25</v>
@@ -2022,22 +2025,23 @@
       <c r="V9" s="6">
         <v>3.94</v>
       </c>
-      <c r="X9" s="6">
+      <c r="W9" s="6"/>
+      <c r="Y9" s="6">
         <v>3</v>
       </c>
-      <c r="Y9" s="6">
+      <c r="Z9" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -2093,25 +2097,28 @@
       <c r="U10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="V10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y10" s="6">
+      <c r="V10" s="6">
+        <v>2.63</v>
+      </c>
+      <c r="W10" s="6">
+        <v>1.31</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z10" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
@@ -2141,7 +2148,7 @@
         <v>100</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>4</v>
@@ -2167,25 +2174,29 @@
       <c r="U11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="V11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="X11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y11" s="6">
+      <c r="V11" s="6">
+        <v>4.13</v>
+      </c>
+      <c r="W11" s="6">
+        <f>5.36-4.13</f>
+        <v>1.2300000000000004</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D12" s="6">
         <v>4</v>
@@ -2215,25 +2226,25 @@
         <v>100</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R12" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T12" s="6" t="s">
         <v>4</v>
@@ -2244,22 +2255,23 @@
       <c r="V12" s="6">
         <v>3.15</v>
       </c>
-      <c r="X12" s="6">
+      <c r="W12" s="6"/>
+      <c r="Y12" s="6">
         <v>6</v>
       </c>
-      <c r="Y12" s="6">
+      <c r="Z12" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D13" s="6">
         <v>6</v>
@@ -2289,28 +2301,28 @@
         <v>150</v>
       </c>
       <c r="M13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="T13" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="S13" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="T13" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="U13" s="6">
         <v>1.07</v>
@@ -2318,22 +2330,23 @@
       <c r="V13" s="6">
         <v>3.15</v>
       </c>
-      <c r="X13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y13" s="6">
+      <c r="W13" s="6"/>
+      <c r="Y13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z13" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D14" s="6">
         <v>3</v>
@@ -2363,7 +2376,7 @@
         <v>100</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N14" s="6" t="s">
         <v>4</v>
@@ -2392,22 +2405,23 @@
       <c r="V14" s="6">
         <v>3.15</v>
       </c>
-      <c r="X14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y14" s="6">
+      <c r="W14" s="6"/>
+      <c r="Y14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D15" s="6">
         <v>2</v>
@@ -2443,22 +2457,22 @@
         <v>4</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>4</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U15" s="6">
         <v>0.79</v>
@@ -2466,22 +2480,23 @@
       <c r="V15" s="6">
         <v>5.95</v>
       </c>
-      <c r="X15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y15" s="6">
+      <c r="W15" s="6"/>
+      <c r="Y15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z15" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D16" s="6">
         <v>4</v>
@@ -2511,25 +2526,25 @@
         <v>100</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="T16" s="6" t="s">
         <v>4</v>
@@ -2537,25 +2552,28 @@
       <c r="U16" s="6">
         <v>0.36</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="X16" s="6">
+      <c r="V16">
+        <v>3.85</v>
+      </c>
+      <c r="W16">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="Y16" s="6">
         <v>6</v>
       </c>
-      <c r="Y16" s="6">
+      <c r="Z16" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D17" s="6">
         <v>3</v>
@@ -2585,25 +2603,25 @@
         <v>60</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="R17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="T17" s="6" t="s">
         <v>4</v>
@@ -2614,22 +2632,23 @@
       <c r="V17" s="6">
         <v>5.6</v>
       </c>
-      <c r="X17" s="6">
-        <v>4</v>
-      </c>
+      <c r="W17" s="6"/>
       <c r="Y17" s="6">
+        <v>4</v>
+      </c>
+      <c r="Z17" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D18" s="6">
         <v>5</v>
@@ -2650,7 +2669,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K18" s="6">
         <v>200</v>
@@ -2659,28 +2678,28 @@
         <v>100</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="O18" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q18" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="S18" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="T18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U18" s="6">
         <v>2.36</v>
@@ -2688,22 +2707,23 @@
       <c r="V18" s="6">
         <v>3.15</v>
       </c>
-      <c r="X18" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y18" s="6">
+      <c r="W18" s="6"/>
+      <c r="Y18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z18" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D19" s="6">
         <v>6</v>
@@ -2724,7 +2744,7 @@
         <v>4</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K19" s="6">
         <v>300</v>
@@ -2733,7 +2753,7 @@
         <v>150</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>4</v>
@@ -2745,10 +2765,10 @@
         <v>4</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="S19" s="6" t="s">
         <v>4</v>
@@ -2763,22 +2783,23 @@
       <c r="V19" s="6">
         <v>2.62</v>
       </c>
-      <c r="X19" s="6">
+      <c r="W19" s="6"/>
+      <c r="Y19" s="6">
         <v>8</v>
       </c>
-      <c r="Y19" s="6">
+      <c r="Z19" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D20" s="6">
         <v>0</v>
@@ -2811,19 +2832,19 @@
         <v>2</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q20" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="S20" s="6" t="s">
         <v>4</v>
@@ -2837,22 +2858,23 @@
       <c r="V20" s="6">
         <v>10.5</v>
       </c>
-      <c r="X20" s="6">
+      <c r="W20" s="6"/>
+      <c r="Y20" s="6">
         <v>2</v>
       </c>
-      <c r="Y20" s="6">
+      <c r="Z20" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D21" s="6">
         <v>8</v>
@@ -2873,7 +2895,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K21" s="6">
         <v>350</v>
@@ -2882,22 +2904,22 @@
         <v>350</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S21" s="6" t="s">
         <v>4</v>
@@ -2911,22 +2933,23 @@
       <c r="V21" s="6">
         <v>2.62</v>
       </c>
-      <c r="X21" s="6">
+      <c r="W21" s="6"/>
+      <c r="Y21" s="6">
         <v>7</v>
       </c>
-      <c r="Y21" s="6">
+      <c r="Z21" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>4</v>
@@ -2941,7 +2964,7 @@
         <v>29</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>4</v>
@@ -2956,7 +2979,7 @@
         <v>150</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="N22" s="6">
         <v>20</v>
@@ -2985,22 +3008,23 @@
       <c r="V22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X22" s="6">
+      <c r="W22" s="6"/>
+      <c r="Y22" s="6">
         <v>7</v>
       </c>
-      <c r="Y22" s="6">
+      <c r="Z22" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -3030,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N23" s="6" t="s">
         <v>3</v>
@@ -3059,22 +3083,23 @@
       <c r="V23" s="6">
         <v>3.94</v>
       </c>
-      <c r="X23" s="6" t="s">
+      <c r="W23" s="6"/>
+      <c r="Y23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Y23" s="6">
+      <c r="Z23" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>4</v>
@@ -3133,22 +3158,23 @@
       <c r="V24" s="6">
         <v>3.94</v>
       </c>
-      <c r="X24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y24" s="6">
+      <c r="W24" s="6"/>
+      <c r="Y24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z24" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
@@ -3181,19 +3207,19 @@
         <v>9</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q25" s="6" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="S25" s="6" t="s">
         <v>4</v>
@@ -3207,22 +3233,23 @@
       <c r="V25" s="6">
         <v>3.15</v>
       </c>
-      <c r="X25" s="6">
+      <c r="W25" s="6"/>
+      <c r="Y25" s="6">
         <v>5</v>
       </c>
-      <c r="Y25" s="6">
+      <c r="Z25" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
@@ -3255,19 +3282,19 @@
         <v>9</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q26" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="S26" s="6" t="s">
         <v>4</v>
@@ -3282,22 +3309,23 @@
         <f>3.15+1.57</f>
         <v>4.72</v>
       </c>
-      <c r="X26" s="6">
+      <c r="W26" s="6"/>
+      <c r="Y26" s="6">
         <v>5</v>
       </c>
-      <c r="Y26" s="6">
+      <c r="Z26" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
@@ -3327,28 +3355,28 @@
         <v>0</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="R27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U27" s="8">
         <v>1.07</v>
@@ -3356,22 +3384,23 @@
       <c r="V27" s="6">
         <v>3.15</v>
       </c>
-      <c r="X27" s="6">
+      <c r="W27" s="6"/>
+      <c r="Y27" s="6">
         <v>6</v>
       </c>
-      <c r="Y27" s="6">
+      <c r="Z27" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
@@ -3401,28 +3430,28 @@
         <v>0</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="R28" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U28" s="6">
         <v>0.71</v>
@@ -3431,22 +3460,23 @@
         <f>3.15+1.57</f>
         <v>4.72</v>
       </c>
-      <c r="X28" s="6">
+      <c r="W28" s="6"/>
+      <c r="Y28" s="6">
         <v>6</v>
       </c>
-      <c r="Y28" s="6">
+      <c r="Z28" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D29" s="6">
         <v>1</v>
@@ -3479,7 +3509,7 @@
         <v>9</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="O29" s="6" t="s">
         <v>4</v>
@@ -3488,7 +3518,7 @@
         <v>4</v>
       </c>
       <c r="Q29" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="R29" s="6" t="s">
         <v>4</v>
@@ -3505,22 +3535,23 @@
       <c r="V29" s="6">
         <v>5.25</v>
       </c>
-      <c r="X29" s="6">
+      <c r="W29" s="6"/>
+      <c r="Y29" s="6">
         <v>5</v>
       </c>
-      <c r="Y29" s="6">
+      <c r="Z29" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D30" s="6">
         <v>2</v>
@@ -3550,25 +3581,25 @@
         <v>0</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="T30" s="6" t="s">
         <v>4</v>
@@ -3579,22 +3610,23 @@
       <c r="V30" s="6">
         <v>3.94</v>
       </c>
-      <c r="X30" s="6">
+      <c r="W30" s="6"/>
+      <c r="Y30" s="6">
         <v>6</v>
       </c>
-      <c r="Y30" s="6">
+      <c r="Z30" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D31" s="6">
         <v>2</v>
@@ -3627,25 +3659,25 @@
         <v>2</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O31" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q31" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R31" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S31" s="6" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="T31" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="U31" s="6">
         <v>1.79</v>
@@ -3653,22 +3685,23 @@
       <c r="V31" s="6">
         <v>5.95</v>
       </c>
-      <c r="X31" s="6">
+      <c r="W31" s="6"/>
+      <c r="Y31" s="6">
         <v>5</v>
       </c>
-      <c r="Y31" s="6">
+      <c r="Z31" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D32" s="6">
         <v>2</v>
@@ -3701,25 +3734,25 @@
         <v>2</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O32" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q32" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="R32" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S32" s="6" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="T32" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="U32" s="6">
         <v>1.79</v>
@@ -3727,22 +3760,23 @@
       <c r="V32" s="6">
         <v>5.95</v>
       </c>
-      <c r="X32" s="6">
+      <c r="W32" s="6"/>
+      <c r="Y32" s="6">
         <v>5</v>
       </c>
-      <c r="Y32" s="6">
+      <c r="Z32" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D33" s="6">
         <v>2</v>
@@ -3772,28 +3806,28 @@
         <v>0</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O33" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Q33" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="R33" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S33" s="6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="T33" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U33" s="6">
         <v>1.43</v>
@@ -3801,22 +3835,23 @@
       <c r="V33" s="6">
         <v>3.15</v>
       </c>
-      <c r="X33" s="6">
+      <c r="W33" s="6"/>
+      <c r="Y33" s="6">
         <v>2</v>
       </c>
-      <c r="Y33" s="6">
+      <c r="Z33" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D34" s="6">
         <v>2</v>
@@ -3846,28 +3881,28 @@
         <v>0</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="R34" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U34" s="6">
         <v>1.43</v>
@@ -3875,22 +3910,23 @@
       <c r="V34" s="6">
         <v>3.15</v>
       </c>
-      <c r="X34" s="6">
+      <c r="W34" s="6"/>
+      <c r="Y34" s="6">
         <v>2</v>
       </c>
-      <c r="Y34" s="6">
+      <c r="Z34" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D35" s="6">
         <v>2</v>
@@ -3929,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q35" s="6" t="s">
         <v>4</v>
@@ -3941,7 +3977,7 @@
         <v>4</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U35" s="6">
         <v>29</v>
@@ -3949,22 +3985,23 @@
       <c r="V35" s="6">
         <v>3.94</v>
       </c>
-      <c r="X35" s="6">
+      <c r="W35" s="6"/>
+      <c r="Y35" s="6">
         <v>5</v>
       </c>
-      <c r="Y35" s="6">
+      <c r="Z35" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D36" s="6">
         <v>3</v>
@@ -3994,25 +4031,25 @@
         <v>0</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="O36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="R36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="T36" s="6" t="s">
         <v>4</v>
@@ -4023,22 +4060,23 @@
       <c r="V36" s="6">
         <v>3.15</v>
       </c>
-      <c r="X36" s="6">
+      <c r="W36" s="6"/>
+      <c r="Y36" s="6">
         <v>7</v>
       </c>
-      <c r="Y36" s="6">
+      <c r="Z36" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D37" s="6">
         <v>3</v>
@@ -4068,28 +4106,28 @@
         <v>0</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O37" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R37" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U37" s="6">
         <v>2.14</v>
@@ -4097,22 +4135,23 @@
       <c r="V37" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X37" s="6">
+      <c r="W37" s="6"/>
+      <c r="Y37" s="6">
         <v>13</v>
       </c>
-      <c r="Y37" s="6">
+      <c r="Z37" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D38" s="6">
         <v>3</v>
@@ -4142,28 +4181,28 @@
         <v>0</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q38" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="R38" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="S38" s="6" t="s">
         <v>4</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U38" s="6">
         <v>0.71</v>
@@ -4171,22 +4210,23 @@
       <c r="V38" s="6">
         <v>4.72</v>
       </c>
-      <c r="X38" s="6">
+      <c r="W38" s="6"/>
+      <c r="Y38" s="6">
         <v>5</v>
       </c>
-      <c r="Y38" s="6">
+      <c r="Z38" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D39" s="6">
         <v>6</v>
@@ -4216,51 +4256,52 @@
         <v>0</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N39" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="S39" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="O39" s="6" t="s">
+      <c r="T39" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="P39" s="6" t="s">
+      <c r="U39" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="Q39" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="R39" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="S39" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="T39" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="U39" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="V39" s="6">
         <v>2.62</v>
       </c>
-      <c r="X39" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y39" s="6">
+      <c r="W39" s="6"/>
+      <c r="Y39" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z39" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D40" s="6">
         <v>6</v>
@@ -4290,28 +4331,28 @@
         <v>0</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="Q40" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="R40" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="S40" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="T40" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="U40" s="6">
         <v>0.91</v>
@@ -4319,22 +4360,23 @@
       <c r="V40" s="6">
         <v>2.62</v>
       </c>
-      <c r="X40" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y40" s="6">
+      <c r="W40" s="6"/>
+      <c r="Y40" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z40" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D41" s="6">
         <v>2</v>
@@ -4364,28 +4406,28 @@
         <v>0</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N41" s="6" t="s">
         <v>4</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="P41" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>4</v>
       </c>
       <c r="R41" s="6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U41" s="6">
         <v>1.43</v>
@@ -4393,22 +4435,23 @@
       <c r="V41" s="6">
         <v>3.85</v>
       </c>
-      <c r="X41" s="6">
+      <c r="W41" s="6"/>
+      <c r="Y41" s="6">
         <v>9</v>
       </c>
-      <c r="Y41" s="6">
+      <c r="Z41" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D42" s="6">
         <v>2</v>
@@ -4438,25 +4481,25 @@
         <v>0</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O42" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P42" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="Q42" s="6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="R42" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S42" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="T42" s="6" t="s">
         <v>4</v>
@@ -4467,22 +4510,23 @@
       <c r="V42" s="6">
         <v>3.15</v>
       </c>
-      <c r="X42" s="6">
+      <c r="W42" s="6"/>
+      <c r="Y42" s="6">
         <v>6</v>
       </c>
-      <c r="Y42" s="6">
+      <c r="Z42" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D43" s="6">
         <v>2</v>
@@ -4512,7 +4556,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>4</v>
@@ -4539,24 +4583,25 @@
         <v>4</v>
       </c>
       <c r="V43" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="X43" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y43" s="6">
+        <v>162</v>
+      </c>
+      <c r="W43" s="6"/>
+      <c r="Y43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z43" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D44" s="6">
         <v>3</v>
@@ -4586,13 +4631,13 @@
         <v>0</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N44" s="6" t="s">
         <v>4</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P44" s="6" t="s">
         <v>4</v>
@@ -4601,13 +4646,13 @@
         <v>4</v>
       </c>
       <c r="R44" s="6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="S44" s="6" t="s">
         <v>4</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U44" s="6">
         <v>1.29</v>
@@ -4615,22 +4660,23 @@
       <c r="V44" s="6">
         <v>4.72</v>
       </c>
-      <c r="X44" s="6">
+      <c r="W44" s="6"/>
+      <c r="Y44" s="6">
         <v>5</v>
       </c>
-      <c r="Y44" s="6">
+      <c r="Z44" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D45" s="6">
         <v>3</v>
@@ -4660,10 +4706,10 @@
         <v>0</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O45" s="6" t="s">
         <v>4</v>
@@ -4672,7 +4718,7 @@
         <v>4</v>
       </c>
       <c r="Q45" s="6" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="R45" s="6" t="s">
         <v>4</v>
@@ -4689,22 +4735,23 @@
       <c r="V45" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X45" s="6" t="s">
-        <v>173</v>
-      </c>
+      <c r="W45" s="6"/>
       <c r="Y45" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="Z45" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D46" s="6">
         <v>3</v>
@@ -4737,7 +4784,7 @@
         <v>2</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="O46" s="6" t="s">
         <v>4</v>
@@ -4746,7 +4793,7 @@
         <v>4</v>
       </c>
       <c r="Q46" s="6" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="R46" s="6" t="s">
         <v>4</v>
@@ -4755,30 +4802,31 @@
         <v>4</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U46" s="6">
         <v>0.89</v>
       </c>
       <c r="V46" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="X46" s="6">
+        <v>172</v>
+      </c>
+      <c r="W46" s="6"/>
+      <c r="Y46" s="6">
         <v>6</v>
       </c>
-      <c r="Y46" s="6">
+      <c r="Z46" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D47" s="6">
         <v>2</v>
@@ -4837,22 +4885,23 @@
       <c r="V47" s="6">
         <v>4.13</v>
       </c>
-      <c r="X47" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y47" s="6">
+      <c r="W47" s="6"/>
+      <c r="Y47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z47" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D48" s="6">
         <v>6</v>
@@ -4873,7 +4922,7 @@
         <v>4</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K48" s="6">
         <v>550</v>
@@ -4882,22 +4931,22 @@
         <v>0</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P48" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q48" s="6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="S48" s="6" t="s">
         <v>4</v>
@@ -4911,22 +4960,23 @@
       <c r="V48" s="6">
         <v>2.62</v>
       </c>
-      <c r="X48" s="6">
+      <c r="W48" s="6"/>
+      <c r="Y48" s="6">
         <v>6</v>
       </c>
-      <c r="Y48" s="6">
+      <c r="Z48" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>4</v>
@@ -4941,13 +4991,13 @@
         <v>36</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="K49" s="6">
         <v>1500</v>
@@ -4956,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="N49" s="6">
         <v>40</v>
@@ -4977,7 +5027,7 @@
         <v>4</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U49" s="6">
         <v>1.43</v>
@@ -4985,22 +5035,23 @@
       <c r="V49" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X49" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y49" s="6">
+      <c r="W49" s="6"/>
+      <c r="Y49" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z49" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>4</v>
@@ -5015,13 +5066,13 @@
         <v>18</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K50" s="6">
         <v>250</v>
@@ -5030,13 +5081,13 @@
         <v>0</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="N50" s="6" t="s">
         <v>4</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="P50" s="6" t="s">
         <v>4</v>
@@ -5059,22 +5110,23 @@
       <c r="V50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X50" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y50" s="6">
+      <c r="W50" s="6"/>
+      <c r="Y50" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z50" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>4</v>
@@ -5089,13 +5141,13 @@
         <v>4</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K51" s="6">
         <v>150</v>
@@ -5104,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="N51" s="6">
         <v>18</v>
@@ -5133,22 +5185,23 @@
       <c r="V51" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="X51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y51" s="6">
+      <c r="W51" s="6"/>
+      <c r="Y51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z51" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>4</v>
@@ -5207,25 +5260,26 @@
       <c r="V52" s="6">
         <v>-0.79</v>
       </c>
-      <c r="W52" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="W52" s="6"/>
       <c r="X52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y52" s="1">
+        <v>189</v>
+      </c>
+      <c r="Y52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z52" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D53" s="6">
         <v>1</v>
@@ -5284,25 +5338,26 @@
       <c r="V53" s="6">
         <v>3.94</v>
       </c>
-      <c r="W53" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="W53" s="6"/>
       <c r="X53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y53" s="1">
+      <c r="Z53" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D54" s="6">
         <v>2</v>
@@ -5332,28 +5387,28 @@
         <v>0</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="P54" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q54" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="R54" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="S54" s="6" t="s">
         <v>4</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U54" s="6">
         <v>0.71</v>
@@ -5361,25 +5416,26 @@
       <c r="V54" s="6">
         <v>1.31</v>
       </c>
-      <c r="W54" s="1" t="s">
-        <v>200</v>
-      </c>
+      <c r="W54" s="6"/>
       <c r="X54" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="Y54" s="1">
+        <v>195</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z54" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D55" s="6">
         <v>0.5</v>
@@ -5412,51 +5468,52 @@
         <v>9</v>
       </c>
       <c r="N55" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U55" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="V55" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="W55" s="6"/>
+      <c r="X55" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z55" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="O55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q55" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="R55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="S55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="T55" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="U55" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="V55" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="W55" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="X55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y55" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>208</v>
-      </c>
       <c r="B56" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D56" s="6">
         <v>0.5</v>
@@ -5480,60 +5537,61 @@
         <v>1</v>
       </c>
       <c r="K56" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P56" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="U56" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="V56" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="W56" s="6"/>
+      <c r="X56" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z56" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="L56" s="2">
-        <v>0</v>
-      </c>
-      <c r="M56" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="N56" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="O56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="P56" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="R56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="S56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="T56" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="U56" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="V56" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="W56" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="X56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y56" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>214</v>
-      </c>
       <c r="B57" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D57" s="6">
         <v>2</v>
@@ -5563,10 +5621,10 @@
         <v>0</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O57" s="6" t="s">
         <v>4</v>
@@ -5575,7 +5633,7 @@
         <v>4</v>
       </c>
       <c r="Q57" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="R57" s="6" t="s">
         <v>4</v>
@@ -5590,27 +5648,28 @@
         <v>1.43</v>
       </c>
       <c r="V57" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="W57" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="X57" s="1">
-        <v>4</v>
+        <v>211</v>
+      </c>
+      <c r="W57" s="6"/>
+      <c r="X57" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="Y57" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z57" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D58" s="6">
         <v>3</v>
@@ -5640,10 +5699,10 @@
         <v>0</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="O58" s="6" t="s">
         <v>4</v>
@@ -5652,7 +5711,7 @@
         <v>4</v>
       </c>
       <c r="Q58" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="R58" s="6" t="s">
         <v>4</v>
@@ -5667,25 +5726,26 @@
       <c r="V58" s="6">
         <v>3.85</v>
       </c>
-      <c r="W58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="X58" s="1">
+      <c r="W58" s="6"/>
+      <c r="X58" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y58" s="1">
         <v>6</v>
       </c>
-      <c r="Y58" s="1">
+      <c r="Z58" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D59" s="6">
         <v>2</v>
@@ -5718,51 +5778,52 @@
         <v>9</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q59" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="R59" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="S59" s="6" t="s">
         <v>4</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U59" s="6">
         <v>0.54</v>
       </c>
       <c r="V59" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="W59" s="1" t="s">
-        <v>207</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="W59" s="6"/>
       <c r="X59" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="Y59" s="1">
+        <v>202</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z59" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D60" s="6">
         <v>3</v>
@@ -5792,54 +5853,55 @@
         <v>0</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="O60" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P60" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="Q60" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="R60" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S60" s="6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="U60" s="6">
         <v>1.43</v>
       </c>
       <c r="V60" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="W60" s="1" t="s">
-        <v>207</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="W60" s="6"/>
       <c r="X60" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="Y60" s="1">
+        <v>202</v>
+      </c>
+      <c r="Y60" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z60" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D61" s="6">
         <v>2</v>
@@ -5869,7 +5931,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="N61" s="6" t="s">
         <v>4</v>
@@ -5898,25 +5960,26 @@
       <c r="V61" s="6">
         <v>3.15</v>
       </c>
-      <c r="W61" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="W61" s="6"/>
       <c r="X61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y61" s="1">
+        <v>202</v>
+      </c>
+      <c r="Y61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z61" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D62" s="6">
         <v>3</v>
@@ -5946,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N62" s="6" t="s">
         <v>4</v>
@@ -5958,7 +6021,7 @@
         <v>4</v>
       </c>
       <c r="Q62" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="R62" s="6" t="s">
         <v>4</v>
@@ -5975,25 +6038,26 @@
       <c r="V62" s="6">
         <v>3.15</v>
       </c>
-      <c r="W62" s="1" t="s">
-        <v>207</v>
-      </c>
+      <c r="W62" s="6"/>
       <c r="X62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y62" s="1">
+        <v>202</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z62" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>4</v>
@@ -6026,7 +6090,7 @@
         <v>9</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O63" s="6" t="s">
         <v>4</v>
@@ -6035,7 +6099,7 @@
         <v>4</v>
       </c>
       <c r="Q63" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R63" s="6" t="s">
         <v>4</v>
@@ -6044,7 +6108,7 @@
         <v>4</v>
       </c>
       <c r="T63" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U63" s="6">
         <v>0.43</v>
@@ -6052,25 +6116,26 @@
       <c r="V63" s="6">
         <v>2.62</v>
       </c>
-      <c r="W63" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="X63" s="1">
+      <c r="W63" s="6"/>
+      <c r="X63" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y63" s="1">
         <v>3</v>
       </c>
-      <c r="Y63" s="1">
+      <c r="Z63" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D64" s="6">
         <v>6</v>
@@ -6091,7 +6156,7 @@
         <v>8</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="K64" s="6">
         <v>500</v>
@@ -6100,10 +6165,10 @@
         <v>0</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="O64" s="6" t="s">
         <v>4</v>
@@ -6112,7 +6177,7 @@
         <v>4</v>
       </c>
       <c r="Q64" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="R64" s="6" t="s">
         <v>4</v>
@@ -6121,33 +6186,34 @@
         <v>4</v>
       </c>
       <c r="T64" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U64" s="6">
         <v>0.61</v>
       </c>
       <c r="V64" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="W64" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="X64" s="1">
+        <v>234</v>
+      </c>
+      <c r="W64" s="6"/>
+      <c r="X64" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y64" s="1">
         <v>1</v>
       </c>
-      <c r="Y64" s="1">
+      <c r="Z64" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>4</v>
@@ -6177,7 +6243,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N65" s="6" t="s">
         <v>4</v>
@@ -6204,27 +6270,28 @@
         <v>4</v>
       </c>
       <c r="V65" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="W65" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="W65" s="6"/>
       <c r="X65" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y65" s="1">
+      <c r="Y65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z65" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>4</v>
@@ -6254,7 +6321,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N66" s="6" t="s">
         <v>4</v>
@@ -6281,27 +6348,28 @@
         <v>4</v>
       </c>
       <c r="V66" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="W66" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="W66" s="6"/>
       <c r="X66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y66" s="1">
+      <c r="Y66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z66" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>4</v>
@@ -6360,25 +6428,26 @@
       <c r="V67" s="6">
         <v>3.15</v>
       </c>
-      <c r="W67" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="W67" s="6"/>
       <c r="X67" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y67" s="1">
+        <v>189</v>
+      </c>
+      <c r="Y67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z67" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D68" s="6">
         <v>2</v>
@@ -6411,25 +6480,25 @@
         <v>9</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>4</v>
       </c>
       <c r="Q68" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="R68" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="S68" s="6" t="s">
         <v>4</v>
       </c>
       <c r="T68" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="U68" s="6">
         <v>1.0900000000000001</v>
@@ -6437,25 +6506,26 @@
       <c r="V68" s="6">
         <v>5.6</v>
       </c>
-      <c r="W68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X68" s="1">
+      <c r="W68" s="6"/>
+      <c r="X68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y68" s="1">
         <v>3</v>
       </c>
-      <c r="Y68" s="1">
+      <c r="Z68" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D69" s="6">
         <v>2</v>
@@ -6476,7 +6546,7 @@
         <v>4</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K69" s="6">
         <v>200</v>
@@ -6485,28 +6555,28 @@
         <v>0</v>
       </c>
       <c r="M69" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="N69" s="6" t="s">
         <v>4</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="Q69" s="6" t="s">
         <v>4</v>
       </c>
       <c r="R69" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="S69" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="T69" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U69" s="6">
         <v>1.36</v>
@@ -6514,25 +6584,26 @@
       <c r="V69" s="6">
         <v>4.7249999999999996</v>
       </c>
-      <c r="W69" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X69" s="1">
+      <c r="W69" s="6"/>
+      <c r="X69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y69" s="1">
         <v>6</v>
       </c>
-      <c r="Y69" s="1">
+      <c r="Z69" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D70" s="6">
         <v>3</v>
@@ -6562,7 +6633,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="N70" s="6" t="s">
         <v>4</v>
@@ -6591,25 +6662,26 @@
       <c r="V70" s="6">
         <v>4.13</v>
       </c>
-      <c r="W70" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="W70" s="6"/>
       <c r="X70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Y70" s="1">
+      <c r="Y70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z70" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D71" s="6">
         <v>4</v>
@@ -6639,10 +6711,10 @@
         <v>0</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="O71" s="6" t="s">
         <v>4</v>
@@ -6651,7 +6723,7 @@
         <v>4</v>
       </c>
       <c r="Q71" s="6" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="R71" s="6" t="s">
         <v>4</v>
@@ -6668,25 +6740,26 @@
       <c r="V71" s="6">
         <v>1.97</v>
       </c>
-      <c r="W71" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X71" s="1">
+      <c r="W71" s="6"/>
+      <c r="X71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y71" s="1">
         <v>10</v>
       </c>
-      <c r="Y71" s="1">
+      <c r="Z71" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>4</v>
@@ -6719,7 +6792,7 @@
         <v>9</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O72" s="6" t="s">
         <v>4</v>
@@ -6728,7 +6801,7 @@
         <v>4</v>
       </c>
       <c r="Q72" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="R72" s="6" t="s">
         <v>4</v>
@@ -6745,25 +6818,26 @@
       <c r="V72" s="6">
         <v>5.37</v>
       </c>
-      <c r="W72" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="W72" s="6"/>
       <c r="X72" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y72" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y72" s="1">
+      <c r="Z72" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>4</v>
@@ -6778,7 +6852,7 @@
         <v>36</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>4</v>
@@ -6793,7 +6867,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="N73" s="6">
         <v>25</v>
@@ -6802,16 +6876,16 @@
         <v>4</v>
       </c>
       <c r="P73" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="Q73" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="R73" s="6" t="s">
         <v>4</v>
       </c>
       <c r="S73" s="6" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="T73" s="6" t="s">
         <v>4</v>
@@ -6819,28 +6893,29 @@
       <c r="U73" s="6">
         <v>1.32</v>
       </c>
-      <c r="V73" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="W73" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="X73" s="1">
+      <c r="V73" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="W73" s="6"/>
+      <c r="X73" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y73" s="1">
         <v>7</v>
       </c>
-      <c r="Y73" s="1">
+      <c r="Z73" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>4</v>
@@ -6855,7 +6930,7 @@
         <v>21</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>4</v>
@@ -6870,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="M74" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="N74" s="6" t="s">
         <v>4</v>
@@ -6879,7 +6954,7 @@
         <v>15</v>
       </c>
       <c r="P74" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="Q74" s="6" t="s">
         <v>4</v>
@@ -6888,24 +6963,25 @@
         <v>24.6</v>
       </c>
       <c r="S74" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="T74" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U74" s="6">
         <v>0.61</v>
       </c>
-      <c r="V74" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="W74" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="X74" s="1">
+      <c r="V74" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="W74" s="6"/>
+      <c r="X74" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y74" s="1">
         <v>7</v>
       </c>
-      <c r="Y74" s="1">
+      <c r="Z74" s="1">
         <v>11</v>
       </c>
     </row>
@@ -6926,71 +7002,70 @@
     <hyperlink ref="A14" r:id="rId13" tooltip="Disruptor" display="https://liquipedia.net/starcraft2/Disruptor"/>
     <hyperlink ref="A15" r:id="rId14" tooltip="Phoenix (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Phoenix_(Legacy_of_the_Void)"/>
     <hyperlink ref="A16" r:id="rId15" tooltip="Void Ray (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Void_Ray_(Legacy_of_the_Void)"/>
-    <hyperlink ref="V16" r:id="rId16" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A17" r:id="rId17" tooltip="Oracle (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Oracle_(Legacy_of_the_Void)"/>
-    <hyperlink ref="N17" r:id="rId18" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A18" r:id="rId19" tooltip="Tempest (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Tempest_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A19" r:id="rId20" tooltip="Carrier (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Carrier_(Legacy_of_the_Void)"/>
-    <hyperlink ref="Q19" r:id="rId21" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
-    <hyperlink ref="U19" r:id="rId22" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A20" r:id="rId23" tooltip="Interceptor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Interceptor_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A21" r:id="rId24" tooltip="Mothership (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Mothership_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A22" r:id="rId25" tooltip="Photon Cannon (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Photon_Cannon_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A23" r:id="rId26" tooltip="SCV (Legacy of the Void)" display="https://liquipedia.net/starcraft2/SCV_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A24" r:id="rId27" tooltip="MULE (Legacy of the Void)" display="https://liquipedia.net/starcraft2/MULE_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A25" r:id="rId28" tooltip="Marine (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marine_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A27" r:id="rId29" tooltip="Marauder (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marauder_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A29" r:id="rId30" tooltip="Reaper (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Reaper_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A30" r:id="rId31" tooltip="Ghost (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Ghost_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A31" r:id="rId32" tooltip="Hellion (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellion_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A34" r:id="rId33" tooltip="Hellbat (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellbat_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A35" r:id="rId34" tooltip="Widow Mine (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Widow_Mine_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A36" r:id="rId35" tooltip="Siege Tank (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Siege_Tank_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A37" r:id="rId36" tooltip="Siege Tank (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Siege_Tank_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A38" r:id="rId37" tooltip="Cyclone" display="https://liquipedia.net/starcraft2/Cyclone"/>
-    <hyperlink ref="A39" r:id="rId38" tooltip="Thor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Thor_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A40" r:id="rId39" tooltip="Thor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Thor_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A41" r:id="rId40" tooltip="Viking (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Viking_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A42" r:id="rId41" tooltip="Viking (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Viking_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A43" r:id="rId42" tooltip="Medivac (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Medivac_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A44" r:id="rId43" tooltip="Liberator" display="https://liquipedia.net/starcraft2/Liberator"/>
-    <hyperlink ref="A45" r:id="rId44" tooltip="Liberator" display="https://liquipedia.net/starcraft2/Liberator"/>
-    <hyperlink ref="A46" r:id="rId45" tooltip="Banshee (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Banshee_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A47" r:id="rId46" tooltip="Raven (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Raven_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A48" r:id="rId47" tooltip="Battlecruiser (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Battlecruiser_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A49" r:id="rId48" tooltip="Planetary Fortress (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Planetary_Fortress_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A50" r:id="rId49" tooltip="Missile Turret (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Missile_Turret_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A51" r:id="rId50" tooltip="Auto-Turret (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Auto-Turret_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A52" r:id="rId51" tooltip="Larva (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Larva_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A53" r:id="rId52" tooltip="Drone (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Drone_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A54" r:id="rId53" tooltip="Queen (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Queen_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A55" r:id="rId54" tooltip="Zergling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Zergling_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A56" r:id="rId55" tooltip="Baneling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Baneling_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A57" r:id="rId56" tooltip="Roach (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Roach_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A58" r:id="rId57" tooltip="Ravager" display="https://liquipedia.net/starcraft2/Ravager"/>
-    <hyperlink ref="A59" r:id="rId58" tooltip="Hydralisk (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hydralisk_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A60" r:id="rId59" tooltip="Lurker (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Lurker_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A61" r:id="rId60" tooltip="Infestor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Infestor_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A62" r:id="rId61" tooltip="Swarm Host (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Swarm_Host_(Legacy_of_the_Void)"/>
-    <hyperlink ref="Q62" r:id="rId62" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A63" r:id="rId63" tooltip="Locust (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Locust_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A64" r:id="rId64" tooltip="Ultralisk (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Ultralisk_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A65" r:id="rId65" tooltip="Overlord (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Overlord_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A66" r:id="rId66" tooltip="Overseer (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Overseer_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A67" r:id="rId67" tooltip="Changeling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Changeling_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A68" r:id="rId68" tooltip="Mutalisk (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Mutalisk_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A69" r:id="rId69" tooltip="Corruptor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Corruptor_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A70" r:id="rId70" tooltip="Viper (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Viper_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A71" r:id="rId71" tooltip="Brood Lord (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Brood_Lord_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A72" r:id="rId72" tooltip="Broodling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Broodling_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A73" r:id="rId73" tooltip="Spine Crawler (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Spine_Crawler_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A74" r:id="rId74" tooltip="Spore Crawler (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Spore_Crawler_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A26" r:id="rId75" tooltip="Marine (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marine_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A28" r:id="rId76" tooltip="Marauder (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marauder_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A32" r:id="rId77" tooltip="Hellion (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellion_(Legacy_of_the_Void)"/>
-    <hyperlink ref="A33" r:id="rId78" tooltip="Hellbat (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellbat_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A17" r:id="rId16" tooltip="Oracle (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Oracle_(Legacy_of_the_Void)"/>
+    <hyperlink ref="N17" r:id="rId17" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A18" r:id="rId18" tooltip="Tempest (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Tempest_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A19" r:id="rId19" tooltip="Carrier (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Carrier_(Legacy_of_the_Void)"/>
+    <hyperlink ref="Q19" r:id="rId20" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
+    <hyperlink ref="U19" r:id="rId21" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A20" r:id="rId22" tooltip="Interceptor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Interceptor_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A21" r:id="rId23" tooltip="Mothership (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Mothership_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A22" r:id="rId24" tooltip="Photon Cannon (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Photon_Cannon_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A23" r:id="rId25" tooltip="SCV (Legacy of the Void)" display="https://liquipedia.net/starcraft2/SCV_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A24" r:id="rId26" tooltip="MULE (Legacy of the Void)" display="https://liquipedia.net/starcraft2/MULE_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A25" r:id="rId27" tooltip="Marine (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marine_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A27" r:id="rId28" tooltip="Marauder (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marauder_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A29" r:id="rId29" tooltip="Reaper (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Reaper_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A30" r:id="rId30" tooltip="Ghost (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Ghost_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A31" r:id="rId31" tooltip="Hellion (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellion_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A34" r:id="rId32" tooltip="Hellbat (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellbat_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A35" r:id="rId33" tooltip="Widow Mine (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Widow_Mine_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A36" r:id="rId34" tooltip="Siege Tank (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Siege_Tank_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A37" r:id="rId35" tooltip="Siege Tank (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Siege_Tank_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A38" r:id="rId36" tooltip="Cyclone" display="https://liquipedia.net/starcraft2/Cyclone"/>
+    <hyperlink ref="A39" r:id="rId37" tooltip="Thor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Thor_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A40" r:id="rId38" tooltip="Thor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Thor_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A41" r:id="rId39" tooltip="Viking (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Viking_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A42" r:id="rId40" tooltip="Viking (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Viking_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A43" r:id="rId41" tooltip="Medivac (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Medivac_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A44" r:id="rId42" tooltip="Liberator" display="https://liquipedia.net/starcraft2/Liberator"/>
+    <hyperlink ref="A45" r:id="rId43" tooltip="Liberator" display="https://liquipedia.net/starcraft2/Liberator"/>
+    <hyperlink ref="A46" r:id="rId44" tooltip="Banshee (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Banshee_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A47" r:id="rId45" tooltip="Raven (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Raven_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A48" r:id="rId46" tooltip="Battlecruiser (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Battlecruiser_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A49" r:id="rId47" tooltip="Planetary Fortress (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Planetary_Fortress_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A50" r:id="rId48" tooltip="Missile Turret (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Missile_Turret_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A51" r:id="rId49" tooltip="Auto-Turret (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Auto-Turret_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A52" r:id="rId50" tooltip="Larva (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Larva_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A53" r:id="rId51" tooltip="Drone (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Drone_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A54" r:id="rId52" tooltip="Queen (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Queen_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A55" r:id="rId53" tooltip="Zergling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Zergling_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A56" r:id="rId54" tooltip="Baneling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Baneling_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A57" r:id="rId55" tooltip="Roach (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Roach_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A58" r:id="rId56" tooltip="Ravager" display="https://liquipedia.net/starcraft2/Ravager"/>
+    <hyperlink ref="A59" r:id="rId57" tooltip="Hydralisk (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hydralisk_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A60" r:id="rId58" tooltip="Lurker (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Lurker_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A61" r:id="rId59" tooltip="Infestor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Infestor_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A62" r:id="rId60" tooltip="Swarm Host (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Swarm_Host_(Legacy_of_the_Void)"/>
+    <hyperlink ref="Q62" r:id="rId61" display="https://liquipedia.net/starcraft2/Unit_Statistics_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A63" r:id="rId62" tooltip="Locust (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Locust_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A64" r:id="rId63" tooltip="Ultralisk (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Ultralisk_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A65" r:id="rId64" tooltip="Overlord (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Overlord_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A66" r:id="rId65" tooltip="Overseer (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Overseer_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A67" r:id="rId66" tooltip="Changeling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Changeling_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A68" r:id="rId67" tooltip="Mutalisk (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Mutalisk_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A69" r:id="rId68" tooltip="Corruptor (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Corruptor_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A70" r:id="rId69" tooltip="Viper (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Viper_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A71" r:id="rId70" tooltip="Brood Lord (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Brood_Lord_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A72" r:id="rId71" tooltip="Broodling (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Broodling_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A73" r:id="rId72" tooltip="Spine Crawler (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Spine_Crawler_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A74" r:id="rId73" tooltip="Spore Crawler (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Spore_Crawler_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A26" r:id="rId74" tooltip="Marine (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marine_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A28" r:id="rId75" tooltip="Marauder (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Marauder_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A32" r:id="rId76" tooltip="Hellion (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellion_(Legacy_of_the_Void)"/>
+    <hyperlink ref="A33" r:id="rId77" tooltip="Hellbat (Legacy of the Void)" display="https://liquipedia.net/starcraft2/Hellbat_(Legacy_of_the_Void)"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
</xml_diff>